<commit_message>
migrated data into ☁︎sql server
</commit_message>
<xml_diff>
--- a/Dataset/data/bus_stops.xlsx
+++ b/Dataset/data/bus_stops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Desktop/Codebase/Assignments/CSC1108-JourneyPlanner/dataset/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06D3AF4-34F9-A148-8C67-FFA38CADD3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F0385C-5491-8A46-A712-8DADF26CF35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
   </bookViews>
@@ -25,14 +25,14 @@
     <sheet name="P411-02" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'P101'!$A$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'P101'!$A$1:$C$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'P102-01'!$A$1:$C$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'P102-02'!$A$1:$C$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'P106'!$A$1:$C$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'P202'!$A$1:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'P106'!$A$1:$C$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'P202'!$A$1:$C$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'P211-01'!$A$1:$C$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'P211-02'!$A$1:$C$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'P403'!$A$1:$C$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'P403'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'P411-01'!$A$1:$C$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'P411-02'!$A$1:$C$36</definedName>
   </definedNames>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="339">
   <si>
     <t>Bus stop</t>
   </si>
@@ -1458,7 +1458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B383786-A1E5-0A42-A2B9-65DCA6F0CA76}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0"/>
   </sheetViews>
@@ -1676,17 +1676,6 @@
       </c>
       <c r="C19" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2099,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C03AD16-751C-B141-A50B-C664EED5BE46}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -2495,17 +2484,6 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <v>33</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2516,7 +2494,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
@@ -2835,17 +2813,6 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2853,7 +2820,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D436B-8365-F94A-8225-647168D0FF6E}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
@@ -3126,17 +3093,6 @@
       </c>
       <c r="C24" s="3" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>